<commit_message>
Modified framework with new URL
</commit_message>
<xml_diff>
--- a/Cucumber/src/test/resources/config/Automation.xlsx
+++ b/Cucumber/src/test/resources/config/Automation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaurav.dixit01\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauravdixit02\git\CucumberFramework-with-Junit\Cucumber\src\test\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576D072E-0337-4680-BE19-4357F8338336}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1303C0C-8274-4692-94A8-E0C3F4CE0CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E076A93F-F130-4FDF-B719-85ADF2F0AB72}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E076A93F-F130-4FDF-B719-85ADF2F0AB72}"/>
   </bookViews>
   <sheets>
     <sheet name="contactus" sheetId="1" r:id="rId1"/>
@@ -34,36 +34,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>subjectheading</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>orderref</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>Webmaster</t>
-  </si>
-  <si>
-    <t>Customer service</t>
-  </si>
-  <si>
     <t>gd@gmail.com</t>
   </si>
   <si>
     <t>guru@gmail.com</t>
   </si>
   <si>
-    <t>Hey GD here</t>
-  </si>
-  <si>
-    <t>Hey Guru here</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>Dixit</t>
+  </si>
+  <si>
+    <t>enquiry</t>
+  </si>
+  <si>
+    <t>doing automation work</t>
+  </si>
+  <si>
+    <t>checking the automation</t>
   </si>
 </sst>
 </file>
@@ -130,9 +127,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -170,7 +167,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -276,7 +273,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -418,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,59 +423,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186DFC25-C41F-4B69-858C-DA5875FB5FA4}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>